<commit_message>
Updated BOM (added components that weren't in the list, corrected values for fuses, ferrite bead)
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="61">
   <si>
     <t>Communication board</t>
   </si>
@@ -174,6 +174,39 @@
   </si>
   <si>
     <t>Tallysman (via Digi Key)</t>
+  </si>
+  <si>
+    <t>Multicomp</t>
+  </si>
+  <si>
+    <t>MC0805B224K500CT</t>
+  </si>
+  <si>
+    <t>0,22uF 0805 50V X7R</t>
+  </si>
+  <si>
+    <t>120R 0603</t>
+  </si>
+  <si>
+    <t>CRCW0603120RFKEA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTC </t>
+  </si>
+  <si>
+    <t>1.1A/1.95A 1812L110/33MR</t>
+  </si>
+  <si>
+    <t>215k 0603</t>
+  </si>
+  <si>
+    <t>CRCW0603215KFKEA</t>
+  </si>
+  <si>
+    <t>5k6 0603</t>
+  </si>
+  <si>
+    <t>mcmr06x5601ftl</t>
   </si>
 </sst>
 </file>
@@ -565,8 +598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,12 +775,35 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="8"/>
-      <c r="D12" s="8"/>
+      <c r="B12" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" s="3">
+        <v>2320842</v>
+      </c>
+      <c r="L12" s="3">
+        <v>8.43E-2</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="8"/>
-      <c r="D13" s="8"/>
+      <c r="B13" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" s="3">
+        <v>1652832</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" s="8"/>
@@ -840,6 +896,57 @@
       </c>
       <c r="L24" s="3">
         <v>0.34599999999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H25" s="3">
+        <v>1822213</v>
+      </c>
+      <c r="L25" s="3">
+        <v>0.70299999999999996</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H26" s="3">
+        <v>2138528</v>
+      </c>
+      <c r="L26" s="3">
+        <v>1.7399999999999999E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H27" s="3">
+        <v>2073537</v>
+      </c>
+      <c r="L27" s="3">
+        <v>8.6999999999999994E-3</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">

</xml_diff>